<commit_message>
organizando pastas de teste
</commit_message>
<xml_diff>
--- a/Holerite.xlsx
+++ b/Holerite.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/b8b2be90b05db14b/Área de Trabalho/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/b8b2be90b05db14b/PROJETO-TI/PROJETOS_PYTHON/codewars-II/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="7" documentId="13_ncr:1_{0D544680-1651-48A1-8D04-58DF2CC179C8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{CA324E6E-71F2-4AF1-9B18-8A1B08850E67}"/>
+  <xr:revisionPtr revIDLastSave="29" documentId="13_ncr:1_{0D544680-1651-48A1-8D04-58DF2CC179C8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F9A3D4E7-FD2D-49F1-8F68-B416FB85A695}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="6" xr2:uid="{0995A3BB-B3C5-470C-8239-7CC4E2D59ED7}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="5" xr2:uid="{0995A3BB-B3C5-470C-8239-7CC4E2D59ED7}"/>
   </bookViews>
   <sheets>
     <sheet name="Instruções" sheetId="7" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="214" uniqueCount="173">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="215" uniqueCount="174">
   <si>
     <t>Código</t>
   </si>
@@ -819,6 +819,9 @@
   </si>
   <si>
     <t xml:space="preserve">  - considerar que estes funcionários não tiveram falta (automaticamente, considerar 22,5 dias trabalhados)</t>
+  </si>
+  <si>
+    <t>total:</t>
   </si>
 </sst>
 </file>
@@ -1122,7 +1125,7 @@
     <xf numFmtId="44" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="87">
+  <cellXfs count="88">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -1284,6 +1287,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Moeda" xfId="1" builtinId="4"/>
@@ -1872,8 +1876,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{88765E50-CFFD-473A-916C-C51016470B04}">
   <dimension ref="A2:G45"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A31" sqref="A1:XFD1048576"/>
+    <sheetView topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="C37" sqref="C32:C37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2190,7 +2194,7 @@
   <dimension ref="A2:G16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD1048576"/>
+      <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2348,7 +2352,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CD1CA19F-3E40-4688-BDF3-1CD167FC187D}">
   <dimension ref="A2:I50"/>
   <sheetViews>
-    <sheetView topLeftCell="A15" workbookViewId="0">
+    <sheetView topLeftCell="A16" workbookViewId="0">
       <selection activeCell="G34" sqref="G34"/>
     </sheetView>
   </sheetViews>
@@ -2825,10 +2829,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C2AB0102-35EF-4E1D-BEC9-2B81BDFBA63E}">
-  <dimension ref="B2:G43"/>
+  <dimension ref="B2:P43"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="D18" sqref="D18"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="M17" sqref="M17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2838,9 +2842,11 @@
     <col min="4" max="4" width="14.140625" customWidth="1"/>
     <col min="5" max="5" width="16.7109375" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="16.140625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="10.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B2" s="77" t="s">
         <v>20</v>
       </c>
@@ -2849,7 +2855,7 @@
       <c r="E2" s="77"/>
       <c r="F2" s="77"/>
     </row>
-    <row r="3" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B3" s="79" t="s">
         <v>21</v>
       </c>
@@ -2864,7 +2870,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="4" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B4" s="79"/>
       <c r="C4" s="45" t="s">
         <v>24</v>
@@ -2875,7 +2881,7 @@
       <c r="E4" s="79"/>
       <c r="F4" s="79"/>
     </row>
-    <row r="5" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B5" s="2">
         <v>1</v>
       </c>
@@ -2891,8 +2897,19 @@
       <c r="F5" s="5">
         <v>0</v>
       </c>
-    </row>
-    <row r="6" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="I5" s="9">
+        <f>D5-C5</f>
+        <v>1212</v>
+      </c>
+      <c r="J5" s="87">
+        <f>E5</f>
+        <v>7.4999999999999997E-2</v>
+      </c>
+      <c r="K5" s="9">
+        <v>90.9</v>
+      </c>
+    </row>
+    <row r="6" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B6" s="2">
         <v>2</v>
       </c>
@@ -2908,8 +2925,19 @@
       <c r="F6" s="5">
         <v>16.5</v>
       </c>
-    </row>
-    <row r="7" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="I6" s="9">
+        <f t="shared" ref="I6:I8" si="0">D6-C6</f>
+        <v>1215.3399999999999</v>
+      </c>
+      <c r="J6" s="87">
+        <f t="shared" ref="J6:J8" si="1">E6</f>
+        <v>0.09</v>
+      </c>
+      <c r="K6" s="9">
+        <v>109.38</v>
+      </c>
+    </row>
+    <row r="7" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B7" s="2">
         <v>3</v>
       </c>
@@ -2925,8 +2953,19 @@
       <c r="F7" s="5">
         <v>82.603999999999999</v>
       </c>
-    </row>
-    <row r="8" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="I7" s="9">
+        <f t="shared" si="0"/>
+        <v>1213.67</v>
+      </c>
+      <c r="J7" s="87">
+        <f t="shared" si="1"/>
+        <v>0.12</v>
+      </c>
+      <c r="K7" s="9">
+        <v>145.63999999999999</v>
+      </c>
+    </row>
+    <row r="8" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B8" s="2">
         <v>4</v>
       </c>
@@ -2942,15 +2981,47 @@
       <c r="F8" s="5">
         <v>148.708</v>
       </c>
-    </row>
-    <row r="9" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="I8" s="9">
+        <f t="shared" si="0"/>
+        <v>3446.1800000000003</v>
+      </c>
+      <c r="J8" s="87">
+        <f t="shared" si="1"/>
+        <v>0.14000000000000001</v>
+      </c>
+      <c r="K8" s="9">
+        <v>482.47</v>
+      </c>
+      <c r="M8" s="9">
+        <f>8000-C8</f>
+        <v>4358.96</v>
+      </c>
+      <c r="N8" s="9">
+        <f>M8*J8</f>
+        <v>610.25440000000003</v>
+      </c>
+      <c r="P8">
+        <v>3446.18</v>
+      </c>
+    </row>
+    <row r="9" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B9" s="47"/>
       <c r="C9" s="48"/>
       <c r="D9" s="48"/>
       <c r="E9" s="49"/>
       <c r="F9" s="50"/>
-    </row>
-    <row r="10" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="J9" t="s">
+        <v>173</v>
+      </c>
+      <c r="K9" s="9">
+        <f>SUM(K5:K8)</f>
+        <v>828.39</v>
+      </c>
+      <c r="P9" s="9">
+        <v>828.38620000000014</v>
+      </c>
+    </row>
+    <row r="10" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B10" s="47"/>
       <c r="C10" t="s">
         <v>36</v>
@@ -2959,7 +3030,7 @@
       <c r="E10" s="49"/>
       <c r="F10" s="50"/>
     </row>
-    <row r="11" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B11" s="47"/>
       <c r="C11" t="s">
         <v>128</v>
@@ -2968,13 +3039,13 @@
       <c r="E11" s="49"/>
       <c r="F11" s="50"/>
     </row>
-    <row r="12" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B12" s="47"/>
       <c r="D12" s="48"/>
       <c r="E12" s="49"/>
       <c r="F12" s="50"/>
     </row>
-    <row r="13" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B13" s="47"/>
       <c r="C13" s="48" t="s">
         <v>129</v>
@@ -2983,7 +3054,7 @@
       <c r="E13" s="49"/>
       <c r="F13" s="50"/>
     </row>
-    <row r="14" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B14" s="47"/>
       <c r="C14" t="s">
         <v>37</v>
@@ -2999,7 +3070,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="15" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:16" x14ac:dyDescent="0.25">
       <c r="E15" t="s">
         <v>82</v>
       </c>
@@ -3257,8 +3328,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0577A86F-4D90-4CA1-B21F-4BBF3A13F06A}">
   <dimension ref="B2:I30"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G9" sqref="G9"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="N22" sqref="N22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
correção valor tabela irrf
</commit_message>
<xml_diff>
--- a/Holerite.xlsx
+++ b/Holerite.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/b8b2be90b05db14b/PROJETO-TI/PROJETOS_PYTHON/codewars-II/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="127" documentId="13_ncr:1_{0D544680-1651-48A1-8D04-58DF2CC179C8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{57E50DA7-DB91-43A2-96AA-A7C9F1E61063}"/>
+  <xr:revisionPtr revIDLastSave="130" documentId="13_ncr:1_{0D544680-1651-48A1-8D04-58DF2CC179C8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F0EB03A8-1C78-4E1F-830B-2D1E6799512C}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="6" xr2:uid="{0995A3BB-B3C5-470C-8239-7CC4E2D59ED7}"/>
   </bookViews>
@@ -1493,16 +1493,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>266700</xdr:colOff>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>142875</xdr:colOff>
       <xdr:row>18</xdr:row>
-      <xdr:rowOff>95250</xdr:rowOff>
+      <xdr:rowOff>85725</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>16</xdr:col>
-      <xdr:colOff>47625</xdr:colOff>
-      <xdr:row>30</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>533400</xdr:colOff>
+      <xdr:row>29</xdr:row>
+      <xdr:rowOff>180975</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -1517,7 +1517,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="6781800" y="3524250"/>
+          <a:off x="4829175" y="3514725"/>
           <a:ext cx="4048125" cy="2190750"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -2571,8 +2571,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CD1CA19F-3E40-4688-BDF3-1CD167FC187D}">
   <dimension ref="A2:I50"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F25" sqref="F25"/>
+    <sheetView topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="C46" sqref="C35:C46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3051,7 +3051,7 @@
   <dimension ref="B2:U43"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="O18" sqref="O18"/>
+      <selection activeCell="R21" sqref="R21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3638,7 +3638,7 @@
   <dimension ref="B2:S30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="S3" sqref="S3:S6"/>
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3691,7 +3691,7 @@
         <v>0</v>
       </c>
       <c r="C5" s="3">
-        <v>1903.88</v>
+        <v>1903.98</v>
       </c>
       <c r="D5" s="8">
         <v>0</v>
@@ -3776,17 +3776,15 @@
       </c>
       <c r="E11" s="82"/>
     </row>
-    <row r="13" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="R13" t="s">
-        <v>176</v>
-      </c>
-      <c r="S13">
-        <v>3090</v>
-      </c>
-    </row>
     <row r="14" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B14" t="s">
         <v>135</v>
+      </c>
+      <c r="R14" t="s">
+        <v>176</v>
+      </c>
+      <c r="S14">
+        <v>3090</v>
       </c>
     </row>
     <row r="15" spans="2:19" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
atualizaççoes preparo para BD
</commit_message>
<xml_diff>
--- a/Holerite.xlsx
+++ b/Holerite.xlsx
@@ -10,7 +10,7 @@
   </mc:AlternateContent>
   <xr:revisionPtr revIDLastSave="130" documentId="13_ncr:1_{0D544680-1651-48A1-8D04-58DF2CC179C8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F0EB03A8-1C78-4E1F-830B-2D1E6799512C}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="6" xr2:uid="{0995A3BB-B3C5-470C-8239-7CC4E2D59ED7}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="4" xr2:uid="{0995A3BB-B3C5-470C-8239-7CC4E2D59ED7}"/>
   </bookViews>
   <sheets>
     <sheet name="Instruções" sheetId="7" r:id="rId1"/>
@@ -2095,8 +2095,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{88765E50-CFFD-473A-916C-C51016470B04}">
   <dimension ref="A2:G45"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="C37" sqref="C32:C37"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I6" sqref="I6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2571,8 +2571,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CD1CA19F-3E40-4688-BDF3-1CD167FC187D}">
   <dimension ref="A2:I50"/>
   <sheetViews>
-    <sheetView topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="C46" sqref="C35:C46"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F51" sqref="F51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3637,8 +3637,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0577A86F-4D90-4CA1-B21F-4BBF3A13F06A}">
   <dimension ref="B2:S30"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="N9" sqref="N9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>